<commit_message>
draw walls for Orange & Greenzone
</commit_message>
<xml_diff>
--- a/Labyrinthe_withnumber.xlsx
+++ b/Labyrinthe_withnumber.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megaport\Desktop\1ARC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\1ARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D33BE8-6ACD-42C5-BF09-0475BCB41D31}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE02C29-75B8-427A-9EC6-D706FE9B5BB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3615" windowWidth="14400" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21420" yWindow="2568" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -555,18 +555,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="BI3" sqref="AY3:BI3"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AR3" sqref="AR3:AV3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="21.9" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="39" width="3" style="1"/>
-    <col min="40" max="61" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="61" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="62" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -708,7 +708,7 @@
       <c r="AU1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AV1" s="10" t="s">
+      <c r="AV1" s="16" t="s">
         <v>5</v>
       </c>
       <c r="AW1" s="10" t="s">
@@ -779,7 +779,7 @@
       <c r="CD1" s="12"/>
       <c r="CE1" s="12"/>
     </row>
-    <row r="2" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -837,7 +837,7 @@
       <c r="AS2" s="12"/>
       <c r="AT2" s="12"/>
       <c r="AU2" s="12"/>
-      <c r="AV2" s="10" t="s">
+      <c r="AV2" s="16" t="s">
         <v>6</v>
       </c>
       <c r="AW2" s="9"/>
@@ -886,7 +886,7 @@
       <c r="CD2" s="12"/>
       <c r="CE2" s="12"/>
     </row>
-    <row r="3" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -994,19 +994,19 @@
       </c>
       <c r="AP3" s="9"/>
       <c r="AQ3" s="9"/>
-      <c r="AR3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AT3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AU3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AV3" s="11" t="s">
+      <c r="AR3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV3" s="17" t="s">
         <v>12</v>
       </c>
       <c r="AW3" s="9"/>
@@ -1073,7 +1073,7 @@
       <c r="CD3" s="12"/>
       <c r="CE3" s="12"/>
     </row>
-    <row r="4" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="AS4" s="12"/>
       <c r="AT4" s="12"/>
       <c r="AU4" s="12"/>
-      <c r="AV4" s="10" t="s">
+      <c r="AV4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="AW4" s="9"/>
@@ -1192,7 +1192,7 @@
       <c r="CD4" s="12"/>
       <c r="CE4" s="12"/>
     </row>
-    <row r="5" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1302,37 +1302,37 @@
       </c>
       <c r="AT5" s="9"/>
       <c r="AU5" s="10"/>
-      <c r="AV5" s="10" t="s">
+      <c r="AV5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AW5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AX5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AY5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AZ5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BA5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BB5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BC5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BD5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BE5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BF5" s="10" t="s">
+      <c r="AW5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BG5" s="9"/>
@@ -1391,7 +1391,7 @@
       <c r="CD5" s="12"/>
       <c r="CE5" s="12"/>
     </row>
-    <row r="6" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="CD6" s="12"/>
       <c r="CE6" s="12"/>
     </row>
-    <row r="7" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
@@ -1679,7 +1679,7 @@
       <c r="CD7" s="12"/>
       <c r="CE7" s="12"/>
     </row>
-    <row r="8" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
@@ -1798,7 +1798,7 @@
       <c r="CD8" s="12"/>
       <c r="CE8" s="12"/>
     </row>
-    <row r="9" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="CD9" s="12"/>
       <c r="CE9" s="12"/>
     </row>
-    <row r="10" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="CD10" s="12"/>
       <c r="CE10" s="12"/>
     </row>
-    <row r="11" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="CD11" s="12"/>
       <c r="CE11" s="12"/>
     </row>
-    <row r="12" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>2</v>
       </c>
@@ -2376,7 +2376,7 @@
       <c r="CD12" s="12"/>
       <c r="CE12" s="12"/>
     </row>
-    <row r="13" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>2</v>
       </c>
@@ -2511,7 +2511,7 @@
       <c r="CD13" s="12"/>
       <c r="CE13" s="12"/>
     </row>
-    <row r="14" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>2</v>
       </c>
@@ -2666,7 +2666,7 @@
       <c r="CD14" s="12"/>
       <c r="CE14" s="12"/>
     </row>
-    <row r="15" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>2</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="CD15" s="12"/>
       <c r="CE15" s="12"/>
     </row>
-    <row r="16" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>2</v>
       </c>
@@ -2962,7 +2962,7 @@
       <c r="CD16" s="12"/>
       <c r="CE16" s="12"/>
     </row>
-    <row r="17" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>2</v>
       </c>
@@ -3073,7 +3073,7 @@
       <c r="CD17" s="12"/>
       <c r="CE17" s="12"/>
     </row>
-    <row r="18" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
@@ -3232,7 +3232,7 @@
       <c r="CD18" s="12"/>
       <c r="CE18" s="12"/>
     </row>
-    <row r="19" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>2</v>
       </c>
@@ -3351,7 +3351,7 @@
       <c r="CD19" s="12"/>
       <c r="CE19" s="12"/>
     </row>
-    <row r="20" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>2</v>
       </c>
@@ -3510,7 +3510,7 @@
       <c r="CD20" s="12"/>
       <c r="CE20" s="12"/>
     </row>
-    <row r="21" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>2</v>
       </c>
@@ -3617,7 +3617,7 @@
       <c r="CD21" s="12"/>
       <c r="CE21" s="12"/>
     </row>
-    <row r="22" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
@@ -3824,7 +3824,7 @@
       <c r="CD22" s="12"/>
       <c r="CE22" s="12"/>
     </row>
-    <row r="23" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -3953,7 +3953,7 @@
       <c r="CD23" s="12"/>
       <c r="CE23" s="12"/>
     </row>
-    <row r="24" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="10"/>
@@ -4038,28 +4038,28 @@
       <c r="CD24" s="12"/>
       <c r="CE24" s="12"/>
     </row>
-    <row r="26" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="28" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AB28" s="2"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
     </row>
-    <row r="29" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AE29" s="2"/>
     </row>
-    <row r="30" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AB30" s="2"/>
       <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
@@ -4068,15 +4068,15 @@
       <c r="AG31" s="2"/>
       <c r="AH31" s="3"/>
     </row>
-    <row r="32" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AE32" s="2"/>
       <c r="AH32" s="2"/>
     </row>
-    <row r="33" spans="28:34" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="28:34" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AE33" s="2"/>
       <c r="AH33" s="2"/>
     </row>
-    <row r="34" spans="28:34" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="28:34" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>

</xml_diff>

<commit_message>
progress draw last zone
</commit_message>
<xml_diff>
--- a/Labyrinthe_withnumber.xlsx
+++ b/Labyrinthe_withnumber.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\1ARC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megaport\Desktop\1ARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE02C29-75B8-427A-9EC6-D706FE9B5BB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B09D948-5394-40D3-B03B-37540AE5997E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21420" yWindow="2568" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3615" windowWidth="14400" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -555,18 +555,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AR3" sqref="AR3:AV3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="21.9" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="39" width="3" style="1"/>
-    <col min="40" max="61" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="61" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="62" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="CD1" s="12"/>
       <c r="CE1" s="12"/>
     </row>
-    <row r="2" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -886,7 +886,7 @@
       <c r="CD2" s="12"/>
       <c r="CE2" s="12"/>
     </row>
-    <row r="3" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="CD3" s="12"/>
       <c r="CE3" s="12"/>
     </row>
-    <row r="4" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1192,7 +1192,7 @@
       <c r="CD4" s="12"/>
       <c r="CE4" s="12"/>
     </row>
-    <row r="5" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1391,7 +1391,7 @@
       <c r="CD5" s="12"/>
       <c r="CE5" s="12"/>
     </row>
-    <row r="6" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="CD6" s="12"/>
       <c r="CE6" s="12"/>
     </row>
-    <row r="7" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>2</v>
       </c>
@@ -1679,7 +1679,7 @@
       <c r="CD7" s="12"/>
       <c r="CE7" s="12"/>
     </row>
-    <row r="8" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
@@ -1798,7 +1798,7 @@
       <c r="CD8" s="12"/>
       <c r="CE8" s="12"/>
     </row>
-    <row r="9" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="CD9" s="12"/>
       <c r="CE9" s="12"/>
     </row>
-    <row r="10" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="CD10" s="12"/>
       <c r="CE10" s="12"/>
     </row>
-    <row r="11" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
@@ -2243,7 +2243,7 @@
       <c r="CD11" s="12"/>
       <c r="CE11" s="12"/>
     </row>
-    <row r="12" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>2</v>
       </c>
@@ -2376,7 +2376,7 @@
       <c r="CD12" s="12"/>
       <c r="CE12" s="12"/>
     </row>
-    <row r="13" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>2</v>
       </c>
@@ -2445,25 +2445,25 @@
       <c r="AN13" s="12"/>
       <c r="AO13" s="12"/>
       <c r="AP13" s="9"/>
-      <c r="AQ13" s="10" t="s">
+      <c r="AQ13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AR13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AT13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AU13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AV13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AW13" s="11" t="s">
+      <c r="AR13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW13" s="17" t="s">
         <v>11</v>
       </c>
       <c r="AX13" s="12"/>
@@ -2471,16 +2471,16 @@
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
       <c r="BB13" s="9"/>
-      <c r="BC13" s="10" t="s">
+      <c r="BC13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="BD13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BE13" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BF13" s="10" t="s">
+      <c r="BD13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF13" s="16" t="s">
         <v>4</v>
       </c>
       <c r="BG13" s="9"/>
@@ -2511,7 +2511,7 @@
       <c r="CD13" s="12"/>
       <c r="CE13" s="12"/>
     </row>
-    <row r="14" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>2</v>
       </c>
@@ -2603,10 +2603,10 @@
       </c>
       <c r="AN14" s="9"/>
       <c r="AO14" s="9"/>
-      <c r="AP14" s="10" t="s">
+      <c r="AP14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AQ14" s="10" t="s">
+      <c r="AQ14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="AR14" s="12"/>
@@ -2614,25 +2614,25 @@
       <c r="AT14" s="10"/>
       <c r="AU14" s="10"/>
       <c r="AV14" s="10"/>
-      <c r="AW14" s="10" t="s">
+      <c r="AW14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AX14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AY14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AZ14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BA14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BB14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BC14" s="10" t="s">
+      <c r="AX14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="BD14" s="9"/>
@@ -2666,7 +2666,7 @@
       <c r="CD14" s="12"/>
       <c r="CE14" s="12"/>
     </row>
-    <row r="15" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>2</v>
       </c>
@@ -2718,13 +2718,13 @@
       <c r="AM15" s="9"/>
       <c r="AN15" s="9"/>
       <c r="AO15" s="9"/>
-      <c r="AP15" s="10" t="s">
+      <c r="AP15" s="16" t="s">
         <v>6</v>
       </c>
       <c r="AQ15" s="9"/>
       <c r="AR15" s="9"/>
       <c r="AS15" s="9"/>
-      <c r="AT15" s="10" t="s">
+      <c r="AT15" s="16" t="s">
         <v>6</v>
       </c>
       <c r="AU15" s="9"/>
@@ -2773,7 +2773,7 @@
       <c r="CD15" s="12"/>
       <c r="CE15" s="12"/>
     </row>
-    <row r="16" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>2</v>
       </c>
@@ -2885,46 +2885,46 @@
       <c r="AO16" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AP16" s="11" t="s">
+      <c r="AP16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AQ16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AR16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AT16" s="11" t="s">
+      <c r="AQ16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="AU16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AV16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AW16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AX16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AY16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AZ16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BA16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BB16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BC16" s="11" t="s">
+      <c r="AU16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC16" s="17" t="s">
         <v>11</v>
       </c>
       <c r="BD16" s="9"/>
@@ -2962,7 +2962,7 @@
       <c r="CD16" s="12"/>
       <c r="CE16" s="12"/>
     </row>
-    <row r="17" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>2</v>
       </c>
@@ -3026,7 +3026,7 @@
       <c r="AQ17" s="9"/>
       <c r="AR17" s="9"/>
       <c r="AS17" s="9"/>
-      <c r="AT17" s="10" t="s">
+      <c r="AT17" s="16" t="s">
         <v>6</v>
       </c>
       <c r="AU17" s="9"/>
@@ -3037,7 +3037,7 @@
       <c r="AZ17" s="9"/>
       <c r="BA17" s="9"/>
       <c r="BB17" s="9"/>
-      <c r="BC17" s="10" t="s">
+      <c r="BC17" s="16" t="s">
         <v>6</v>
       </c>
       <c r="BD17" s="9"/>
@@ -3073,7 +3073,7 @@
       <c r="CD17" s="12"/>
       <c r="CE17" s="12"/>
     </row>
-    <row r="18" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
@@ -3177,26 +3177,26 @@
       </c>
       <c r="AR18" s="9"/>
       <c r="AS18" s="9"/>
-      <c r="AT18" s="10" t="s">
+      <c r="AT18" s="16" t="s">
         <v>6</v>
       </c>
       <c r="AU18" s="9"/>
       <c r="AV18" s="10"/>
-      <c r="AW18" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AX18" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AY18" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AZ18" s="11" t="s">
+      <c r="AW18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY18" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ18" s="17" t="s">
         <v>11</v>
       </c>
       <c r="BA18" s="9"/>
       <c r="BB18" s="9"/>
-      <c r="BC18" s="10" t="s">
+      <c r="BC18" s="16" t="s">
         <v>6</v>
       </c>
       <c r="BD18" s="9"/>
@@ -3232,7 +3232,7 @@
       <c r="CD18" s="12"/>
       <c r="CE18" s="12"/>
     </row>
-    <row r="19" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>2</v>
       </c>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="AR19" s="9"/>
       <c r="AS19" s="9"/>
-      <c r="AT19" s="10" t="s">
+      <c r="AT19" s="16" t="s">
         <v>6</v>
       </c>
       <c r="AU19" s="9"/>
@@ -3310,12 +3310,12 @@
       <c r="AY19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AZ19" s="10" t="s">
+      <c r="AZ19" s="16" t="s">
         <v>6</v>
       </c>
       <c r="BA19" s="9"/>
       <c r="BB19" s="9"/>
-      <c r="BC19" s="10" t="s">
+      <c r="BC19" s="16" t="s">
         <v>6</v>
       </c>
       <c r="BD19" s="9"/>
@@ -3351,7 +3351,7 @@
       <c r="CD19" s="12"/>
       <c r="CE19" s="12"/>
     </row>
-    <row r="20" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>2</v>
       </c>
@@ -3451,30 +3451,30 @@
       </c>
       <c r="AR20" s="9"/>
       <c r="AS20" s="9"/>
-      <c r="AT20" s="10" t="s">
+      <c r="AT20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AU20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AV20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AW20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AX20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AY20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AZ20" s="10" t="s">
+      <c r="AU20" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV20" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW20" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX20" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY20" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ20" s="16" t="s">
         <v>10</v>
       </c>
       <c r="BA20" s="10"/>
       <c r="BB20" s="10"/>
-      <c r="BC20" s="10" t="s">
+      <c r="BC20" s="16" t="s">
         <v>6</v>
       </c>
       <c r="BD20" s="9"/>
@@ -3510,7 +3510,7 @@
       <c r="CD20" s="12"/>
       <c r="CE20" s="12"/>
     </row>
-    <row r="21" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>2</v>
       </c>
@@ -3583,7 +3583,7 @@
       <c r="AZ21" s="9"/>
       <c r="BA21" s="9"/>
       <c r="BB21" s="9"/>
-      <c r="BC21" s="10" t="s">
+      <c r="BC21" s="16" t="s">
         <v>6</v>
       </c>
       <c r="BD21" s="9"/>
@@ -3617,7 +3617,7 @@
       <c r="CD21" s="12"/>
       <c r="CE21" s="12"/>
     </row>
-    <row r="22" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="BB22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="BC22" s="11" t="s">
+      <c r="BC22" s="17" t="s">
         <v>13</v>
       </c>
       <c r="BD22" s="10" t="s">
@@ -3824,7 +3824,7 @@
       <c r="CD22" s="12"/>
       <c r="CE22" s="12"/>
     </row>
-    <row r="23" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -3953,7 +3953,7 @@
       <c r="CD23" s="12"/>
       <c r="CE23" s="12"/>
     </row>
-    <row r="24" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="10"/>
@@ -4038,28 +4038,28 @@
       <c r="CD24" s="12"/>
       <c r="CE24" s="12"/>
     </row>
-    <row r="26" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="28" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AB28" s="2"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
     </row>
-    <row r="29" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AE29" s="2"/>
     </row>
-    <row r="30" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AB30" s="2"/>
       <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
@@ -4068,15 +4068,15 @@
       <c r="AG31" s="2"/>
       <c r="AH31" s="3"/>
     </row>
-    <row r="32" spans="1:83" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:83" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AE32" s="2"/>
       <c r="AH32" s="2"/>
     </row>
-    <row r="33" spans="28:34" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="28:34" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AE33" s="2"/>
       <c r="AH33" s="2"/>
     </row>
-    <row r="34" spans="28:34" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="28:34" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>

</xml_diff>

<commit_message>
add error to fix
</commit_message>
<xml_diff>
--- a/Labyrinthe_withnumber.xlsx
+++ b/Labyrinthe_withnumber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\1ARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979989E0-AC73-44FC-8793-BA817ACE19F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD4670B-99E3-46FA-82AA-7EC4B721E515}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7404" yWindow="2208" windowWidth="23052" windowHeight="12384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +173,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -186,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,6 +244,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI21" sqref="AI21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BC17" sqref="BC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="21.9" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -951,7 +963,7 @@
       <c r="X3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Y3" s="19" t="s">
         <v>4</v>
       </c>
       <c r="Z3" s="16" t="s">
@@ -1201,7 +1213,7 @@
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -2294,13 +2306,13 @@
       <c r="X12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Y12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA12" s="10" t="s">
+      <c r="Y12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA12" s="16" t="s">
         <v>4</v>
       </c>
       <c r="AB12" s="9"/>
@@ -2472,7 +2484,7 @@
       <c r="AY13" s="10"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
-      <c r="BB13" s="9"/>
+      <c r="BB13" s="18"/>
       <c r="BC13" s="16" t="s">
         <v>7</v>
       </c>

</xml_diff>